<commit_message>
Updated macroinverts_site_trends code to calculate crustacea site trends. There was a problem with convergence. it is now solved.
</commit_message>
<xml_diff>
--- a/Tables/Winners and losers.xlsx
+++ b/Tables/Winners and losers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\OneDrive\University of Johannesburg\Post-Doc\Nature Research Centre\How Changes in Bioversity Change Biodiversity\Analyses\Biochange_Paper1\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40436072c29b51f3/University of Johannesburg/Post-Doc/Nature Research Centre/How Changes in Bioversity Change Biodiversity/Analyses/Biochange_Paper1/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8EEC35DE-C3AA-4B80-A1B1-5AC238258F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{8EEC35DE-C3AA-4B80-A1B1-5AC238258F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBCA9238-1352-47BE-83F9-6CD8253E103A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LT_2010-2020_winners_losers" sheetId="1" r:id="rId1"/>
@@ -379,7 +379,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -904,39 +904,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -976,72 +944,18 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1354,12 +1268,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="C97" sqref="C97:D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1714,54 +1628,54 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>101</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
       <c r="E14">
-        <v>0.54463555316817402</v>
+        <v>0.83113143497841702</v>
       </c>
       <c r="F14">
-        <v>0.19410092040500401</v>
+        <v>0.19223479671378199</v>
       </c>
       <c r="G14">
-        <v>2.80594008535228</v>
+        <v>4.3235223236711304</v>
       </c>
       <c r="H14">
-        <v>3.0921037642821399E-2</v>
+        <v>4.9636081194334896E-3</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
       <c r="E15">
-        <v>0.51983844126753598</v>
+        <v>0.78906580519522196</v>
       </c>
       <c r="F15">
-        <v>0.118278469014271</v>
+        <v>0.158033239827714</v>
       </c>
       <c r="G15">
-        <v>4.3950386372080397</v>
+        <v>4.99303694624912</v>
       </c>
       <c r="H15">
-        <v>4.5929110056047396E-3</v>
+        <v>2.4694103470981601E-3</v>
       </c>
     </row>
     <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -1870,28 +1784,28 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>11</v>
       </c>
       <c r="E20">
-        <v>0.78906580519522196</v>
+        <v>0.68929312594376502</v>
       </c>
       <c r="F20">
-        <v>0.158033239827714</v>
+        <v>0.20573552274975701</v>
       </c>
       <c r="G20">
-        <v>4.99303694624912</v>
+        <v>3.3503845944104298</v>
       </c>
       <c r="H20">
-        <v>2.4694103470981601E-3</v>
+        <v>1.54120274948568E-2</v>
       </c>
     </row>
     <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -2000,28 +1914,28 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>92</v>
+        <v>11</v>
       </c>
       <c r="E25">
-        <v>0.83113143497841702</v>
+        <v>0.561421889362126</v>
       </c>
       <c r="F25">
-        <v>0.19223479671378199</v>
+        <v>0.18390961197351999</v>
       </c>
       <c r="G25">
-        <v>4.3235223236711304</v>
+        <v>3.05270552929534</v>
       </c>
       <c r="H25">
-        <v>4.9636081194334896E-3</v>
+        <v>2.2433901387577299E-2</v>
       </c>
     </row>
     <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -2052,54 +1966,54 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
       </c>
       <c r="E27">
-        <v>0.68929312594376502</v>
+        <v>0.54463555316817402</v>
       </c>
       <c r="F27">
-        <v>0.20573552274975701</v>
+        <v>0.19410092040500401</v>
       </c>
       <c r="G27">
-        <v>3.3503845944104298</v>
+        <v>2.80594008535228</v>
       </c>
       <c r="H27">
-        <v>1.54120274948568E-2</v>
+        <v>3.0921037642821399E-2</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
       </c>
       <c r="E28">
-        <v>0.561421889362126</v>
+        <v>0.51983844126753598</v>
       </c>
       <c r="F28">
-        <v>0.18390961197351999</v>
+        <v>0.118278469014271</v>
       </c>
       <c r="G28">
-        <v>3.05270552929534</v>
+        <v>4.3950386372080397</v>
       </c>
       <c r="H28">
-        <v>2.2433901387577299E-2</v>
+        <v>4.5929110056047396E-3</v>
       </c>
     </row>
     <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -2156,54 +2070,54 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="E31">
-        <v>0.325531979834289</v>
+        <v>0.50168801604344804</v>
       </c>
       <c r="F31">
-        <v>7.7906772922242296E-2</v>
+        <v>0.162138927139166</v>
       </c>
       <c r="G31">
-        <v>4.1784811207518304</v>
+        <v>3.09418610876117</v>
       </c>
       <c r="H31">
-        <v>5.8233204260532698E-3</v>
+        <v>2.1273787909486599E-2</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="E32">
-        <v>0.451573228588869</v>
+        <v>0.465795081972178</v>
       </c>
       <c r="F32">
-        <v>0.12963199001894399</v>
+        <v>0.12394569109513801</v>
       </c>
       <c r="G32">
-        <v>3.4835014761624699</v>
+        <v>3.7580578869389201</v>
       </c>
       <c r="H32">
-        <v>1.30865346087601E-2</v>
+        <v>9.4200167695272403E-3</v>
       </c>
     </row>
     <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -2286,10 +2200,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C36" t="s">
         <v>67</v>
@@ -2298,16 +2212,16 @@
         <v>67</v>
       </c>
       <c r="E36">
-        <v>0.50168801604344804</v>
+        <v>0.45226498317090302</v>
       </c>
       <c r="F36">
-        <v>0.162138927139166</v>
+        <v>0.17144534442329501</v>
       </c>
       <c r="G36">
-        <v>3.09418610876117</v>
+        <v>2.6379542978680699</v>
       </c>
       <c r="H36">
-        <v>2.1273787909486599E-2</v>
+        <v>3.8646046871036698E-2</v>
       </c>
     </row>
     <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -2520,28 +2434,28 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="C45" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="D45" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="E45">
-        <v>0.45226498317090302</v>
+        <v>0.451573228588869</v>
       </c>
       <c r="F45">
-        <v>0.17144534442329501</v>
+        <v>0.12963199001894399</v>
       </c>
       <c r="G45">
-        <v>2.6379542978680699</v>
+        <v>3.4835014761624699</v>
       </c>
       <c r="H45">
-        <v>3.8646046871036698E-2</v>
+        <v>1.30865346087601E-2</v>
       </c>
     </row>
     <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -2624,7 +2538,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B49" t="s">
         <v>66</v>
@@ -2636,42 +2550,42 @@
         <v>67</v>
       </c>
       <c r="E49">
-        <v>0.465795081972178</v>
+        <v>0.445081073667769</v>
       </c>
       <c r="F49">
-        <v>0.12394569109513801</v>
+        <v>0.131762756239937</v>
       </c>
       <c r="G49">
-        <v>3.7580578869389201</v>
+        <v>3.37789741478454</v>
       </c>
       <c r="H49">
-        <v>9.4200167695272403E-3</v>
+        <v>1.4896414526541699E-2</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="B50" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="C50" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="E50">
-        <v>0.445081073667769</v>
+        <v>0.325531979834289</v>
       </c>
       <c r="F50">
-        <v>0.131762756239937</v>
+        <v>7.7906772922242296E-2</v>
       </c>
       <c r="G50">
-        <v>3.37789741478454</v>
+        <v>4.1784811207518304</v>
       </c>
       <c r="H50">
-        <v>1.4896414526541699E-2</v>
+        <v>5.8233204260532698E-3</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
@@ -3248,80 +3162,80 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="B73" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="C73" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D73" t="s">
-        <v>92</v>
+        <v>11</v>
       </c>
       <c r="E73">
-        <v>-0.52868002804702297</v>
+        <v>-0.19874197561659901</v>
       </c>
       <c r="F73">
-        <v>8.8609096090950107E-2</v>
+        <v>7.3422601563665896E-2</v>
       </c>
       <c r="G73">
-        <v>-5.9664306642331102</v>
+        <v>-2.7068228499676099</v>
       </c>
       <c r="H73">
-        <v>9.933320415794881E-4</v>
+        <v>3.52546551321401E-2</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B74" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="D74" t="s">
         <v>11</v>
       </c>
       <c r="E74">
-        <v>-0.45560770483472302</v>
+        <v>-0.27515933011931598</v>
       </c>
       <c r="F74">
-        <v>0.114381169543175</v>
+        <v>0.108986489432307</v>
       </c>
       <c r="G74">
-        <v>-3.9832404814041098</v>
+        <v>-2.52471046230204</v>
       </c>
       <c r="H74">
-        <v>7.2563442583151103E-3</v>
+        <v>4.4999901845836202E-2</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="D75" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="E75">
-        <v>-0.27515933011931598</v>
+        <v>-0.32424329015784797</v>
       </c>
       <c r="F75">
-        <v>0.108986489432307</v>
+        <v>0.114139577742882</v>
       </c>
       <c r="G75">
-        <v>-2.52471046230204</v>
+        <v>-2.84076125538382</v>
       </c>
       <c r="H75">
-        <v>4.4999901845836202E-2</v>
+        <v>2.9537426681000001E-2</v>
       </c>
     </row>
     <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -3404,7 +3318,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B79" t="s">
         <v>9</v>
@@ -3416,16 +3330,16 @@
         <v>11</v>
       </c>
       <c r="E79">
-        <v>-0.45746593112061601</v>
+        <v>-0.429168836049034</v>
       </c>
       <c r="F79">
-        <v>0.10203570374357</v>
+        <v>0.16057273157857699</v>
       </c>
       <c r="G79">
-        <v>-4.4833907577125203</v>
+        <v>-2.6727379663403101</v>
       </c>
       <c r="H79">
-        <v>4.1772482985172896E-3</v>
+        <v>3.6891607180086002E-2</v>
       </c>
     </row>
     <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -3456,28 +3370,28 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B81" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="C81" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="D81" t="s">
         <v>11</v>
       </c>
       <c r="E81">
-        <v>-0.429168836049034</v>
+        <v>-0.45560770483472302</v>
       </c>
       <c r="F81">
-        <v>0.16057273157857699</v>
+        <v>0.114381169543175</v>
       </c>
       <c r="G81">
-        <v>-2.6727379663403101</v>
+        <v>-3.9832404814041098</v>
       </c>
       <c r="H81">
-        <v>3.6891607180086002E-2</v>
+        <v>7.2563442583151103E-3</v>
       </c>
     </row>
     <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -3638,10 +3552,10 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B88" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C88" t="s">
         <v>10</v>
@@ -3650,16 +3564,16 @@
         <v>11</v>
       </c>
       <c r="E88">
-        <v>-0.59855935858146803</v>
+        <v>-0.45746593112061601</v>
       </c>
       <c r="F88">
-        <v>0.107556401048693</v>
+        <v>0.10203570374357</v>
       </c>
       <c r="G88">
-        <v>-5.5650742563474997</v>
+        <v>-4.4833907577125203</v>
       </c>
       <c r="H88">
-        <v>1.4260700227059801E-3</v>
+        <v>4.1772482985172896E-3</v>
       </c>
     </row>
     <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -3690,66 +3604,66 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="B90" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="C90" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="D90" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="E90">
-        <v>-0.32424329015784797</v>
+        <v>-0.52868002804702297</v>
       </c>
       <c r="F90">
-        <v>0.114139577742882</v>
+        <v>8.8609096090950107E-2</v>
       </c>
       <c r="G90">
-        <v>-2.84076125538382</v>
+        <v>-5.9664306642331102</v>
       </c>
       <c r="H90">
-        <v>2.9537426681000001E-2</v>
+        <v>9.933320415794881E-4</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>113</v>
+        <v>37</v>
       </c>
       <c r="B91" t="s">
-        <v>110</v>
+        <v>33</v>
       </c>
       <c r="C91" t="s">
-        <v>104</v>
+        <v>10</v>
       </c>
       <c r="D91" t="s">
         <v>11</v>
       </c>
       <c r="E91">
-        <v>-0.19874197561659901</v>
+        <v>-0.59855935858146803</v>
       </c>
       <c r="F91">
-        <v>7.3422601563665896E-2</v>
+        <v>0.107556401048693</v>
       </c>
       <c r="G91">
-        <v>-2.7068228499676099</v>
+        <v>-5.5650742563474997</v>
       </c>
       <c r="H91">
-        <v>3.52546551321401E-2</v>
+        <v>1.4260700227059801E-3</v>
       </c>
     </row>
     <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <autoFilter ref="A1:H94">
+  <autoFilter ref="A1:H94" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="7">
-      <colorFilter dxfId="2"/>
+      <colorFilter dxfId="5"/>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:H91">
-      <sortCondition sortBy="cellColor" ref="E1:E94" dxfId="1"/>
+      <sortCondition descending="1" ref="E1:E94"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H94">
@@ -3757,18 +3671,18 @@
     <sortCondition ref="D2:D94"/>
     <sortCondition ref="B2:B94"/>
     <sortCondition ref="A2:A94"/>
-    <sortCondition sortBy="cellColor" ref="E2:E94" dxfId="3"/>
+    <sortCondition sortBy="cellColor" ref="E2:E94" dxfId="4"/>
   </sortState>
   <conditionalFormatting sqref="E2:E91">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H91">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>